<commit_message>
Even MOre files xD
</commit_message>
<xml_diff>
--- a/Excel-Python-Automation/try1/INPUT.xlsx
+++ b/Excel-Python-Automation/try1/INPUT.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\rish project\try1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\rish project\Excel-Python-Automation\try1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2907CB1-7827-46F0-BF1E-F930BF332B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E70DA4-9167-4761-8408-67380C7F30CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -137,7 +137,7 @@
     <t>NPV</t>
   </si>
   <si>
-    <t>ME!Rk1</t>
+    <t>Shobhan Dude</t>
   </si>
 </sst>
 </file>
@@ -390,25 +390,31 @@
     <xf numFmtId="10" fontId="1" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -418,12 +424,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -710,7 +710,7 @@
   <dimension ref="A2:V56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -840,16 +840,16 @@
       <c r="V14" s="23"/>
     </row>
     <row r="16" spans="1:22" ht="21" x14ac:dyDescent="0.5">
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
       <c r="K16" s="13" t="s">
         <v>25</v>
       </c>
@@ -858,25 +858,25 @@
       <c r="C17" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="36">
+      <c r="D17" s="27">
         <v>0</v>
       </c>
-      <c r="E17" s="36">
+      <c r="E17" s="27">
         <v>1</v>
       </c>
-      <c r="F17" s="36">
+      <c r="F17" s="27">
         <v>2</v>
       </c>
-      <c r="G17" s="36">
+      <c r="G17" s="27">
         <v>3</v>
       </c>
-      <c r="H17" s="36">
+      <c r="H17" s="27">
         <v>4</v>
       </c>
-      <c r="I17" s="36">
+      <c r="I17" s="27">
         <v>5</v>
       </c>
-      <c r="J17" s="36">
+      <c r="J17" s="27">
         <v>6</v>
       </c>
     </row>
@@ -884,13 +884,13 @@
       <c r="C18" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
     </row>
     <row r="19" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C19" s="8" t="s">
@@ -915,7 +915,7 @@
       <c r="J19" s="20">
         <v>2656.34</v>
       </c>
-      <c r="K19" s="31" t="s">
+      <c r="K19" s="29" t="s">
         <v>1</v>
       </c>
     </row>
@@ -942,7 +942,7 @@
       <c r="J20" s="20">
         <v>501.16</v>
       </c>
-      <c r="K20" s="31"/>
+      <c r="K20" s="29"/>
     </row>
     <row r="21" spans="3:19" ht="29" x14ac:dyDescent="0.35">
       <c r="C21" s="8" t="s">
@@ -1142,16 +1142,16 @@
       <c r="J29" s="2"/>
     </row>
     <row r="30" spans="3:19" ht="21" x14ac:dyDescent="0.5">
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
     </row>
     <row r="31" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C31" s="8" t="s">
@@ -1188,40 +1188,40 @@
       </c>
     </row>
     <row r="35" spans="3:11" ht="21" x14ac:dyDescent="0.5">
-      <c r="C35" s="27" t="s">
+      <c r="C35" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="27"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="26"/>
     </row>
     <row r="36" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C36" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D36" s="36">
+      <c r="D36" s="27">
         <v>0</v>
       </c>
-      <c r="E36" s="36">
+      <c r="E36" s="27">
         <v>1</v>
       </c>
-      <c r="F36" s="36">
+      <c r="F36" s="27">
         <v>2</v>
       </c>
-      <c r="G36" s="36">
+      <c r="G36" s="27">
         <v>3</v>
       </c>
-      <c r="H36" s="36">
+      <c r="H36" s="27">
         <v>4</v>
       </c>
-      <c r="I36" s="36">
+      <c r="I36" s="27">
         <v>5</v>
       </c>
-      <c r="J36" s="36">
+      <c r="J36" s="27">
         <v>6</v>
       </c>
     </row>
@@ -1229,13 +1229,13 @@
       <c r="C37" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D37" s="37"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="37"/>
-      <c r="H37" s="37"/>
-      <c r="I37" s="37"/>
-      <c r="J37" s="37"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="28"/>
+      <c r="I37" s="28"/>
+      <c r="J37" s="28"/>
     </row>
     <row r="38" spans="3:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C38" s="8" t="s">
@@ -1414,81 +1414,81 @@
       <c r="J45" s="8"/>
     </row>
     <row r="48" spans="3:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="C48" s="32" t="s">
+      <c r="C48" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="D48" s="32"/>
-      <c r="E48" s="32"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="32"/>
-      <c r="H48" s="32"/>
-      <c r="I48" s="32"/>
-      <c r="J48" s="32"/>
+      <c r="D48" s="34"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="34"/>
+      <c r="G48" s="34"/>
+      <c r="H48" s="34"/>
+      <c r="I48" s="34"/>
+      <c r="J48" s="34"/>
       <c r="K48" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="49" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C49" s="8"/>
-      <c r="D49" s="30" t="s">
+      <c r="D49" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E49" s="29"/>
-      <c r="F49" s="30" t="s">
+      <c r="E49" s="32"/>
+      <c r="F49" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="G49" s="29"/>
-      <c r="H49" s="30" t="s">
+      <c r="G49" s="32"/>
+      <c r="H49" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="I49" s="28"/>
-      <c r="J49" s="29"/>
+      <c r="I49" s="31"/>
+      <c r="J49" s="32"/>
     </row>
     <row r="50" spans="3:11" ht="29" x14ac:dyDescent="0.35">
       <c r="C50" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D50" s="33">
+      <c r="D50" s="35">
         <v>2</v>
       </c>
-      <c r="E50" s="34"/>
-      <c r="F50" s="33">
+      <c r="E50" s="36"/>
+      <c r="F50" s="35">
         <v>2</v>
       </c>
-      <c r="G50" s="34"/>
-      <c r="H50" s="33">
+      <c r="G50" s="36"/>
+      <c r="H50" s="35">
         <v>2</v>
       </c>
-      <c r="I50" s="35"/>
-      <c r="J50" s="34"/>
+      <c r="I50" s="37"/>
+      <c r="J50" s="36"/>
       <c r="K50" s="11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="53" spans="3:11" ht="21" x14ac:dyDescent="0.5">
-      <c r="C53" s="26" t="s">
+      <c r="C53" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="D53" s="27"/>
-      <c r="E53" s="27"/>
-      <c r="F53" s="27"/>
-      <c r="G53" s="27"/>
-      <c r="H53" s="27"/>
-      <c r="I53" s="27"/>
-      <c r="J53" s="26"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="26"/>
+      <c r="G53" s="26"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="26"/>
+      <c r="J53" s="30"/>
     </row>
     <row r="54" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C54" s="10"/>
-      <c r="D54" s="28" t="s">
+      <c r="D54" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E54" s="28"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="30" t="s">
+      <c r="E54" s="31"/>
+      <c r="F54" s="32"/>
+      <c r="G54" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="H54" s="28"/>
-      <c r="I54" s="28"/>
+      <c r="H54" s="31"/>
+      <c r="I54" s="31"/>
       <c r="J54" s="10"/>
     </row>
     <row r="55" spans="3:11" x14ac:dyDescent="0.35">
@@ -1512,7 +1512,7 @@
         <v>2</v>
       </c>
       <c r="J55" s="6"/>
-      <c r="K55" s="31" t="s">
+      <c r="K55" s="29" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1539,28 +1539,10 @@
         <v>412.53</v>
       </c>
       <c r="J56" s="3"/>
-      <c r="K56" s="31"/>
+      <c r="K56" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C16:J16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="C30:J30"/>
-    <mergeCell ref="C35:J35"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="H36:H37"/>
-    <mergeCell ref="I36:I37"/>
-    <mergeCell ref="J36:J37"/>
     <mergeCell ref="C53:J53"/>
     <mergeCell ref="D54:F54"/>
     <mergeCell ref="G54:I54"/>
@@ -1572,6 +1554,24 @@
     <mergeCell ref="D50:E50"/>
     <mergeCell ref="F50:G50"/>
     <mergeCell ref="H50:J50"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="C30:J30"/>
+    <mergeCell ref="C35:J35"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="H36:H37"/>
+    <mergeCell ref="I36:I37"/>
+    <mergeCell ref="J36:J37"/>
+    <mergeCell ref="C16:J16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>